<commit_message>
added list of imaged isolates
</commit_message>
<xml_diff>
--- a/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
+++ b/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah 23\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha.gcupadhaya\OneDrive - Washington State University (email.wsu.edu)\Desktop\LabDocuments\FungalCulture\VdIsolatesList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B0C038-6CDE-4A05-A7A8-D0E45E32B633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{02B0C038-6CDE-4A05-A7A8-D0E45E32B633}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B0473D5-148E-44C1-B927-D56B99351831}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Recultured 2021" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Imaged" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8054" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8304" uniqueCount="1399">
   <si>
     <t>Plate</t>
   </si>
@@ -4247,6 +4248,21 @@
   </si>
   <si>
     <t>Vt.USDA29</t>
+  </si>
+  <si>
+    <t>Oct_2020</t>
+  </si>
+  <si>
+    <t>2B (4B)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>HSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Hyperspectral images of these isolates are already taken on October 2020. </t>
   </si>
 </sst>
 </file>
@@ -4351,7 +4367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4484,6 +4500,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -4517,7 +4551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4938,6 +4972,44 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5220,8 +5292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1141"/>
   <sheetViews>
-    <sheetView topLeftCell="A289" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C290" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G316" sqref="G316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31874,8 +31946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8ED01F-2F3E-43EB-B954-6EDC9D012A16}">
   <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33537,8 +33609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2726E2F-E8EA-472C-A800-F178F067C4BF}">
   <dimension ref="A1:E1135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A499" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E505" sqref="E505"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49594,4 +49666,1914 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAB2BD6-6402-43B4-8817-A6E2ACF3D94A}">
+  <dimension ref="A1:W31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="146">
+        <v>10</v>
+      </c>
+      <c r="B3" s="146">
+        <v>1</v>
+      </c>
+      <c r="C3" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="147">
+        <v>52</v>
+      </c>
+      <c r="E3" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K3" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N3" s="146">
+        <v>28</v>
+      </c>
+      <c r="O3" s="146">
+        <v>13</v>
+      </c>
+      <c r="P3" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="146">
+        <v>15</v>
+      </c>
+      <c r="R3" s="146">
+        <v>28</v>
+      </c>
+      <c r="S3" s="146">
+        <v>19</v>
+      </c>
+      <c r="T3" s="146">
+        <v>29</v>
+      </c>
+      <c r="U3" s="146">
+        <v>5</v>
+      </c>
+      <c r="V3" s="146">
+        <v>4</v>
+      </c>
+      <c r="W3" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="146">
+        <v>16</v>
+      </c>
+      <c r="B4" s="146">
+        <v>1</v>
+      </c>
+      <c r="C4" s="146" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="147">
+        <v>74</v>
+      </c>
+      <c r="E4" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K4" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N4" s="146">
+        <v>28</v>
+      </c>
+      <c r="O4" s="146">
+        <v>13</v>
+      </c>
+      <c r="P4" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="146">
+        <v>15</v>
+      </c>
+      <c r="R4" s="146">
+        <v>28</v>
+      </c>
+      <c r="S4" s="146">
+        <v>19</v>
+      </c>
+      <c r="T4" s="146">
+        <v>29</v>
+      </c>
+      <c r="U4" s="146">
+        <v>5</v>
+      </c>
+      <c r="V4" s="146">
+        <v>4</v>
+      </c>
+      <c r="W4" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="146">
+        <v>17</v>
+      </c>
+      <c r="B5" s="146">
+        <v>1</v>
+      </c>
+      <c r="C5" s="146" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="147">
+        <v>103</v>
+      </c>
+      <c r="E5" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K5" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N5" s="146">
+        <v>28</v>
+      </c>
+      <c r="O5" s="146">
+        <v>13</v>
+      </c>
+      <c r="P5" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="146">
+        <v>15</v>
+      </c>
+      <c r="R5" s="146">
+        <v>28</v>
+      </c>
+      <c r="S5" s="146">
+        <v>19</v>
+      </c>
+      <c r="T5" s="146">
+        <v>29</v>
+      </c>
+      <c r="U5" s="146">
+        <v>5</v>
+      </c>
+      <c r="V5" s="146">
+        <v>4</v>
+      </c>
+      <c r="W5" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="146">
+        <v>18</v>
+      </c>
+      <c r="B6" s="146">
+        <v>1</v>
+      </c>
+      <c r="C6" s="146" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="147">
+        <v>104</v>
+      </c>
+      <c r="E6" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K6" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N6" s="146">
+        <v>28</v>
+      </c>
+      <c r="O6" s="146">
+        <v>13</v>
+      </c>
+      <c r="P6" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="146">
+        <v>15</v>
+      </c>
+      <c r="R6" s="146">
+        <v>28</v>
+      </c>
+      <c r="S6" s="146">
+        <v>19</v>
+      </c>
+      <c r="T6" s="146">
+        <v>29</v>
+      </c>
+      <c r="U6" s="146">
+        <v>5</v>
+      </c>
+      <c r="V6" s="146">
+        <v>4</v>
+      </c>
+      <c r="W6" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="146">
+        <v>19</v>
+      </c>
+      <c r="B7" s="146">
+        <v>1</v>
+      </c>
+      <c r="C7" s="146" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="147">
+        <v>121</v>
+      </c>
+      <c r="E7" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K7" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N7" s="146">
+        <v>28</v>
+      </c>
+      <c r="O7" s="146">
+        <v>13</v>
+      </c>
+      <c r="P7" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="146">
+        <v>15</v>
+      </c>
+      <c r="R7" s="146">
+        <v>28</v>
+      </c>
+      <c r="S7" s="146">
+        <v>19</v>
+      </c>
+      <c r="T7" s="146">
+        <v>29</v>
+      </c>
+      <c r="U7" s="146">
+        <v>5</v>
+      </c>
+      <c r="V7" s="146">
+        <v>4</v>
+      </c>
+      <c r="W7" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="146">
+        <v>37</v>
+      </c>
+      <c r="B8" s="146">
+        <v>1</v>
+      </c>
+      <c r="C8" s="146" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="147">
+        <v>80</v>
+      </c>
+      <c r="E8" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="146" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="146" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K8" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N8" s="146">
+        <v>28</v>
+      </c>
+      <c r="O8" s="146">
+        <v>13</v>
+      </c>
+      <c r="P8" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="146">
+        <v>15</v>
+      </c>
+      <c r="R8" s="146">
+        <v>28</v>
+      </c>
+      <c r="S8" s="146">
+        <v>19</v>
+      </c>
+      <c r="T8" s="146">
+        <v>29</v>
+      </c>
+      <c r="U8" s="146">
+        <v>5</v>
+      </c>
+      <c r="V8" s="146">
+        <v>4</v>
+      </c>
+      <c r="W8" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="146">
+        <v>61</v>
+      </c>
+      <c r="B9" s="146">
+        <v>1</v>
+      </c>
+      <c r="C9" s="146" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="147">
+        <v>111</v>
+      </c>
+      <c r="E9" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="146" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="146" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K9" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N9" s="146">
+        <v>28</v>
+      </c>
+      <c r="O9" s="146">
+        <v>13</v>
+      </c>
+      <c r="P9" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="146">
+        <v>15</v>
+      </c>
+      <c r="R9" s="146">
+        <v>28</v>
+      </c>
+      <c r="S9" s="146">
+        <v>19</v>
+      </c>
+      <c r="T9" s="146">
+        <v>29</v>
+      </c>
+      <c r="U9" s="146">
+        <v>5</v>
+      </c>
+      <c r="V9" s="146">
+        <v>4</v>
+      </c>
+      <c r="W9" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="146">
+        <v>69</v>
+      </c>
+      <c r="B10" s="146">
+        <v>1</v>
+      </c>
+      <c r="C10" s="146" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="147">
+        <v>45</v>
+      </c>
+      <c r="E10" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="146" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K10" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N10" s="146">
+        <v>28</v>
+      </c>
+      <c r="O10" s="146">
+        <v>13</v>
+      </c>
+      <c r="P10" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="146">
+        <v>15</v>
+      </c>
+      <c r="R10" s="146">
+        <v>28</v>
+      </c>
+      <c r="S10" s="146">
+        <v>19</v>
+      </c>
+      <c r="T10" s="146">
+        <v>29</v>
+      </c>
+      <c r="U10" s="146">
+        <v>5</v>
+      </c>
+      <c r="V10" s="146">
+        <v>4</v>
+      </c>
+      <c r="W10" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="146">
+        <v>72</v>
+      </c>
+      <c r="B11" s="146">
+        <v>2</v>
+      </c>
+      <c r="C11" s="146" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="147">
+        <v>62</v>
+      </c>
+      <c r="E11" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="146" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="146">
+        <v>1996</v>
+      </c>
+      <c r="K11" s="146" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N11" s="146">
+        <v>28</v>
+      </c>
+      <c r="O11" s="146">
+        <v>13</v>
+      </c>
+      <c r="P11" s="146">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="146">
+        <v>15</v>
+      </c>
+      <c r="R11" s="146">
+        <v>28</v>
+      </c>
+      <c r="S11" s="146">
+        <v>19</v>
+      </c>
+      <c r="T11" s="146">
+        <v>29</v>
+      </c>
+      <c r="U11" s="146">
+        <v>5</v>
+      </c>
+      <c r="V11" s="146">
+        <v>4</v>
+      </c>
+      <c r="W11" s="146">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="148">
+        <v>120</v>
+      </c>
+      <c r="B12" s="148">
+        <v>4</v>
+      </c>
+      <c r="C12" s="148" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="149" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="148" t="s">
+        <v>179</v>
+      </c>
+      <c r="I12" s="148" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K12" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N12" s="148">
+        <v>25</v>
+      </c>
+      <c r="O12" s="148">
+        <v>9</v>
+      </c>
+      <c r="P12" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="148">
+        <v>13</v>
+      </c>
+      <c r="R12" s="148">
+        <v>27</v>
+      </c>
+      <c r="S12" s="148">
+        <v>16</v>
+      </c>
+      <c r="T12" s="148">
+        <v>5</v>
+      </c>
+      <c r="U12" s="148">
+        <v>2</v>
+      </c>
+      <c r="V12" s="148">
+        <v>2</v>
+      </c>
+      <c r="W12" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="148">
+        <v>122</v>
+      </c>
+      <c r="B13" s="148">
+        <v>3</v>
+      </c>
+      <c r="C13" s="148" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="149">
+        <v>653</v>
+      </c>
+      <c r="E13" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="148" t="s">
+        <v>191</v>
+      </c>
+      <c r="I13" s="148" t="s">
+        <v>145</v>
+      </c>
+      <c r="J13" s="148">
+        <v>1995</v>
+      </c>
+      <c r="K13" s="148" t="s">
+        <v>192</v>
+      </c>
+      <c r="L13" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N13" s="148">
+        <v>25</v>
+      </c>
+      <c r="O13" s="148">
+        <v>9</v>
+      </c>
+      <c r="P13" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="148">
+        <v>13</v>
+      </c>
+      <c r="R13" s="148">
+        <v>27</v>
+      </c>
+      <c r="S13" s="148">
+        <v>16</v>
+      </c>
+      <c r="T13" s="148">
+        <v>5</v>
+      </c>
+      <c r="U13" s="148">
+        <v>2</v>
+      </c>
+      <c r="V13" s="148">
+        <v>2</v>
+      </c>
+      <c r="W13" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="148">
+        <v>152</v>
+      </c>
+      <c r="B14" s="148">
+        <v>4</v>
+      </c>
+      <c r="C14" s="148" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="149" t="s">
+        <v>236</v>
+      </c>
+      <c r="E14" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="148" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="148" t="s">
+        <v>237</v>
+      </c>
+      <c r="I14" s="148" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K14" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L14" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M14" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N14" s="148">
+        <v>25</v>
+      </c>
+      <c r="O14" s="148">
+        <v>9</v>
+      </c>
+      <c r="P14" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="148">
+        <v>13</v>
+      </c>
+      <c r="R14" s="148">
+        <v>27</v>
+      </c>
+      <c r="S14" s="148">
+        <v>16</v>
+      </c>
+      <c r="T14" s="148">
+        <v>5</v>
+      </c>
+      <c r="U14" s="148">
+        <v>2</v>
+      </c>
+      <c r="V14" s="148">
+        <v>2</v>
+      </c>
+      <c r="W14" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="148">
+        <v>156</v>
+      </c>
+      <c r="B15" s="148">
+        <v>4</v>
+      </c>
+      <c r="C15" s="148" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="149" t="s">
+        <v>242</v>
+      </c>
+      <c r="E15" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="148" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="I15" s="148" t="s">
+        <v>145</v>
+      </c>
+      <c r="J15" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K15" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L15" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M15" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N15" s="148">
+        <v>25</v>
+      </c>
+      <c r="O15" s="148">
+        <v>9</v>
+      </c>
+      <c r="P15" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="148">
+        <v>13</v>
+      </c>
+      <c r="R15" s="148">
+        <v>27</v>
+      </c>
+      <c r="S15" s="148">
+        <v>16</v>
+      </c>
+      <c r="T15" s="148">
+        <v>5</v>
+      </c>
+      <c r="U15" s="148">
+        <v>2</v>
+      </c>
+      <c r="V15" s="148">
+        <v>2</v>
+      </c>
+      <c r="W15" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="148">
+        <v>183</v>
+      </c>
+      <c r="B16" s="148">
+        <v>4</v>
+      </c>
+      <c r="C16" s="148" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="149" t="s">
+        <v>282</v>
+      </c>
+      <c r="E16" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="I16" s="148" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K16" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L16" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M16" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N16" s="148">
+        <v>25</v>
+      </c>
+      <c r="O16" s="148">
+        <v>9</v>
+      </c>
+      <c r="P16" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="148">
+        <v>13</v>
+      </c>
+      <c r="R16" s="148">
+        <v>27</v>
+      </c>
+      <c r="S16" s="148">
+        <v>16</v>
+      </c>
+      <c r="T16" s="148">
+        <v>5</v>
+      </c>
+      <c r="U16" s="148">
+        <v>2</v>
+      </c>
+      <c r="V16" s="148">
+        <v>2</v>
+      </c>
+      <c r="W16" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="148">
+        <v>184</v>
+      </c>
+      <c r="B17" s="148">
+        <v>4</v>
+      </c>
+      <c r="C17" s="148" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="149" t="s">
+        <v>283</v>
+      </c>
+      <c r="E17" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="J17" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K17" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L17" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M17" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N17" s="148">
+        <v>25</v>
+      </c>
+      <c r="O17" s="148">
+        <v>9</v>
+      </c>
+      <c r="P17" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="148">
+        <v>13</v>
+      </c>
+      <c r="R17" s="148">
+        <v>27</v>
+      </c>
+      <c r="S17" s="148">
+        <v>16</v>
+      </c>
+      <c r="T17" s="148">
+        <v>5</v>
+      </c>
+      <c r="U17" s="148">
+        <v>2</v>
+      </c>
+      <c r="V17" s="148">
+        <v>2</v>
+      </c>
+      <c r="W17" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="148">
+        <v>200</v>
+      </c>
+      <c r="B18" s="148">
+        <v>3</v>
+      </c>
+      <c r="C18" s="148" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="149" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="148" t="s">
+        <v>143</v>
+      </c>
+      <c r="H18" s="148" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" s="148" t="s">
+        <v>145</v>
+      </c>
+      <c r="J18" s="148">
+        <v>2007</v>
+      </c>
+      <c r="K18" s="148" t="s">
+        <v>146</v>
+      </c>
+      <c r="L18" s="148" t="s">
+        <v>168</v>
+      </c>
+      <c r="M18" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N18" s="148">
+        <v>25</v>
+      </c>
+      <c r="O18" s="148">
+        <v>9</v>
+      </c>
+      <c r="P18" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="148">
+        <v>13</v>
+      </c>
+      <c r="R18" s="148">
+        <v>27</v>
+      </c>
+      <c r="S18" s="148">
+        <v>16</v>
+      </c>
+      <c r="T18" s="148">
+        <v>5</v>
+      </c>
+      <c r="U18" s="148">
+        <v>2</v>
+      </c>
+      <c r="V18" s="148">
+        <v>2</v>
+      </c>
+      <c r="W18" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="148">
+        <v>217</v>
+      </c>
+      <c r="B19" s="148">
+        <v>4</v>
+      </c>
+      <c r="C19" s="148" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="149" t="s">
+        <v>337</v>
+      </c>
+      <c r="E19" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="148" t="s">
+        <v>191</v>
+      </c>
+      <c r="G19" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="H19" s="148" t="s">
+        <v>226</v>
+      </c>
+      <c r="I19" s="148" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K19" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L19" s="148" t="s">
+        <v>336</v>
+      </c>
+      <c r="M19" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N19" s="148">
+        <v>24</v>
+      </c>
+      <c r="O19" s="148">
+        <v>9</v>
+      </c>
+      <c r="P19" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="148">
+        <v>13</v>
+      </c>
+      <c r="R19" s="148">
+        <v>27</v>
+      </c>
+      <c r="S19" s="148">
+        <v>16</v>
+      </c>
+      <c r="T19" s="148">
+        <v>5</v>
+      </c>
+      <c r="U19" s="148">
+        <v>2</v>
+      </c>
+      <c r="V19" s="148">
+        <v>2</v>
+      </c>
+      <c r="W19" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="150">
+        <v>224</v>
+      </c>
+      <c r="B20" s="150">
+        <v>2</v>
+      </c>
+      <c r="C20" s="150" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20" s="151" t="s">
+        <v>348</v>
+      </c>
+      <c r="E20" s="150" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F20" s="150" t="s">
+        <v>350</v>
+      </c>
+      <c r="H20" s="150" t="s">
+        <v>351</v>
+      </c>
+      <c r="I20" s="150" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="150">
+        <v>2001</v>
+      </c>
+      <c r="K20" s="150" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" s="150" t="s">
+        <v>352</v>
+      </c>
+      <c r="M20" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N20" s="150">
+        <v>24</v>
+      </c>
+      <c r="O20" s="150">
+        <v>14</v>
+      </c>
+      <c r="P20" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="150">
+        <v>11</v>
+      </c>
+      <c r="R20" s="150">
+        <v>30</v>
+      </c>
+      <c r="S20" s="150">
+        <v>16</v>
+      </c>
+      <c r="T20" s="150">
+        <v>5</v>
+      </c>
+      <c r="U20" s="150">
+        <v>2</v>
+      </c>
+      <c r="V20" s="150">
+        <v>10</v>
+      </c>
+      <c r="W20" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="150">
+        <v>226</v>
+      </c>
+      <c r="B21" s="150">
+        <v>2</v>
+      </c>
+      <c r="C21" s="150" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="151">
+        <v>239</v>
+      </c>
+      <c r="E21" s="150" t="s">
+        <v>343</v>
+      </c>
+      <c r="F21" s="150" t="s">
+        <v>179</v>
+      </c>
+      <c r="I21" s="150" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="150">
+        <v>1995</v>
+      </c>
+      <c r="K21" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="L21" s="150" t="s">
+        <v>352</v>
+      </c>
+      <c r="M21" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N21" s="150">
+        <v>24</v>
+      </c>
+      <c r="O21" s="150">
+        <v>14</v>
+      </c>
+      <c r="P21" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="150">
+        <v>11</v>
+      </c>
+      <c r="R21" s="150">
+        <v>30</v>
+      </c>
+      <c r="S21" s="150">
+        <v>16</v>
+      </c>
+      <c r="T21" s="150">
+        <v>5</v>
+      </c>
+      <c r="U21" s="150">
+        <v>2</v>
+      </c>
+      <c r="V21" s="150">
+        <v>10</v>
+      </c>
+      <c r="W21" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="150">
+        <v>230</v>
+      </c>
+      <c r="B22" s="150">
+        <v>4</v>
+      </c>
+      <c r="C22" s="150" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="151" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" s="150" t="s">
+        <v>343</v>
+      </c>
+      <c r="F22" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="150" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="I22" s="150" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="150">
+        <v>2010</v>
+      </c>
+      <c r="K22" s="150" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="150" t="s">
+        <v>352</v>
+      </c>
+      <c r="M22" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N22" s="150">
+        <v>24</v>
+      </c>
+      <c r="O22" s="150">
+        <v>14</v>
+      </c>
+      <c r="P22" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="150">
+        <v>11</v>
+      </c>
+      <c r="R22" s="150">
+        <v>30</v>
+      </c>
+      <c r="S22" s="150">
+        <v>16</v>
+      </c>
+      <c r="T22" s="150">
+        <v>5</v>
+      </c>
+      <c r="U22" s="150">
+        <v>2</v>
+      </c>
+      <c r="V22" s="150">
+        <v>10</v>
+      </c>
+      <c r="W22" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="150">
+        <v>235</v>
+      </c>
+      <c r="B23" s="150">
+        <v>3</v>
+      </c>
+      <c r="C23" s="150" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="151">
+        <v>235</v>
+      </c>
+      <c r="E23" s="150" t="s">
+        <v>343</v>
+      </c>
+      <c r="F23" s="150" t="s">
+        <v>179</v>
+      </c>
+      <c r="I23" s="150" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="150">
+        <v>1995</v>
+      </c>
+      <c r="K23" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="L23" s="150" t="s">
+        <v>362</v>
+      </c>
+      <c r="M23" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N23" s="150">
+        <v>24</v>
+      </c>
+      <c r="O23" s="150">
+        <v>15</v>
+      </c>
+      <c r="P23" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="150">
+        <v>11</v>
+      </c>
+      <c r="R23" s="150">
+        <v>30</v>
+      </c>
+      <c r="S23" s="150">
+        <v>16</v>
+      </c>
+      <c r="T23" s="150">
+        <v>5</v>
+      </c>
+      <c r="U23" s="150">
+        <v>2</v>
+      </c>
+      <c r="V23" s="150">
+        <v>4</v>
+      </c>
+      <c r="W23" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="150">
+        <v>245</v>
+      </c>
+      <c r="B24" s="150">
+        <v>4</v>
+      </c>
+      <c r="C24" s="150" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="151" t="s">
+        <v>374</v>
+      </c>
+      <c r="E24" s="150" t="s">
+        <v>343</v>
+      </c>
+      <c r="F24" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="G24" s="150" t="s">
+        <v>375</v>
+      </c>
+      <c r="H24" s="150" t="s">
+        <v>226</v>
+      </c>
+      <c r="I24" s="150" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="150">
+        <v>2010</v>
+      </c>
+      <c r="K24" s="150" t="s">
+        <v>120</v>
+      </c>
+      <c r="L24" s="150" t="s">
+        <v>369</v>
+      </c>
+      <c r="M24" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N24" s="150">
+        <v>25</v>
+      </c>
+      <c r="O24" s="150">
+        <v>14</v>
+      </c>
+      <c r="P24" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="150">
+        <v>11</v>
+      </c>
+      <c r="R24" s="150">
+        <v>30</v>
+      </c>
+      <c r="S24" s="150">
+        <v>16</v>
+      </c>
+      <c r="T24" s="150">
+        <v>5</v>
+      </c>
+      <c r="U24" s="150">
+        <v>2</v>
+      </c>
+      <c r="V24" s="150">
+        <v>10</v>
+      </c>
+      <c r="W24" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="150">
+        <v>252</v>
+      </c>
+      <c r="B25" s="150">
+        <v>4</v>
+      </c>
+      <c r="C25" s="150" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="151" t="s">
+        <v>387</v>
+      </c>
+      <c r="E25" s="150" t="s">
+        <v>343</v>
+      </c>
+      <c r="F25" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="G25" s="150" t="s">
+        <v>234</v>
+      </c>
+      <c r="H25" s="150" t="s">
+        <v>235</v>
+      </c>
+      <c r="I25" s="150" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="150">
+        <v>2010</v>
+      </c>
+      <c r="K25" s="150" t="s">
+        <v>120</v>
+      </c>
+      <c r="L25" s="150" t="s">
+        <v>388</v>
+      </c>
+      <c r="M25" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N25" s="150">
+        <v>24</v>
+      </c>
+      <c r="O25" s="150">
+        <v>9</v>
+      </c>
+      <c r="P25" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="150">
+        <v>11</v>
+      </c>
+      <c r="R25" s="150">
+        <v>30</v>
+      </c>
+      <c r="S25" s="150">
+        <v>16</v>
+      </c>
+      <c r="T25" s="150">
+        <v>5</v>
+      </c>
+      <c r="U25" s="150">
+        <v>2</v>
+      </c>
+      <c r="V25" s="150">
+        <v>10</v>
+      </c>
+      <c r="W25" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="150">
+        <v>258</v>
+      </c>
+      <c r="B26" s="150">
+        <v>2</v>
+      </c>
+      <c r="C26" s="150" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="151">
+        <v>240</v>
+      </c>
+      <c r="E26" s="150" t="s">
+        <v>343</v>
+      </c>
+      <c r="F26" s="150" t="s">
+        <v>179</v>
+      </c>
+      <c r="I26" s="150" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="150" t="s">
+        <v>402</v>
+      </c>
+      <c r="K26" s="150" t="s">
+        <v>403</v>
+      </c>
+      <c r="L26" s="150" t="s">
+        <v>404</v>
+      </c>
+      <c r="M26" s="150" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N26" s="150">
+        <v>25</v>
+      </c>
+      <c r="O26" s="150">
+        <v>15</v>
+      </c>
+      <c r="P26" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="150">
+        <v>11</v>
+      </c>
+      <c r="R26" s="150">
+        <v>30</v>
+      </c>
+      <c r="S26" s="150">
+        <v>16</v>
+      </c>
+      <c r="T26" s="150">
+        <v>5</v>
+      </c>
+      <c r="U26" s="150">
+        <v>2</v>
+      </c>
+      <c r="V26" s="150">
+        <v>2</v>
+      </c>
+      <c r="W26" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" s="148" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="148">
+        <v>260</v>
+      </c>
+      <c r="B27" s="148">
+        <v>4</v>
+      </c>
+      <c r="C27" s="148" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="149" t="s">
+        <v>408</v>
+      </c>
+      <c r="E27" s="148" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="148" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="148" t="s">
+        <v>234</v>
+      </c>
+      <c r="H27" s="148" t="s">
+        <v>235</v>
+      </c>
+      <c r="I27" s="148" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="148">
+        <v>2010</v>
+      </c>
+      <c r="K27" s="148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L27" s="148" t="s">
+        <v>409</v>
+      </c>
+      <c r="M27" s="148" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N27" s="148">
+        <v>26</v>
+      </c>
+      <c r="O27" s="148">
+        <v>9</v>
+      </c>
+      <c r="P27" s="148">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="148">
+        <v>13</v>
+      </c>
+      <c r="R27" s="148">
+        <v>27</v>
+      </c>
+      <c r="S27" s="148">
+        <v>16</v>
+      </c>
+      <c r="T27" s="148">
+        <v>5</v>
+      </c>
+      <c r="U27" s="148">
+        <v>2</v>
+      </c>
+      <c r="V27" s="148">
+        <v>2</v>
+      </c>
+      <c r="W27" s="148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="152">
+        <v>286</v>
+      </c>
+      <c r="B28" s="152">
+        <v>3</v>
+      </c>
+      <c r="C28" s="152" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="153" t="s">
+        <v>459</v>
+      </c>
+      <c r="E28" s="152" t="s">
+        <v>460</v>
+      </c>
+      <c r="F28" s="152" t="s">
+        <v>461</v>
+      </c>
+      <c r="K28" s="152" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="152" t="s">
+        <v>462</v>
+      </c>
+      <c r="M28" s="152" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N28" s="152">
+        <v>22</v>
+      </c>
+      <c r="O28" s="152">
+        <v>8</v>
+      </c>
+      <c r="P28" s="152">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="152">
+        <v>15</v>
+      </c>
+      <c r="R28" s="152">
+        <v>27</v>
+      </c>
+      <c r="S28" s="152">
+        <v>19</v>
+      </c>
+      <c r="T28" s="152">
+        <v>8</v>
+      </c>
+      <c r="U28" s="152">
+        <v>2</v>
+      </c>
+      <c r="V28" s="152">
+        <v>3</v>
+      </c>
+      <c r="W28" s="152">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" s="146" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="154">
+        <v>1</v>
+      </c>
+      <c r="C29" s="154" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="155">
+        <v>57</v>
+      </c>
+      <c r="E29" s="156" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="156" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="156"/>
+      <c r="H29" s="156" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="157" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="158">
+        <v>1996</v>
+      </c>
+      <c r="K29" s="159" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="158" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="146" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N29" s="158">
+        <v>28</v>
+      </c>
+      <c r="O29" s="160">
+        <v>13</v>
+      </c>
+      <c r="P29" s="160">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="84">
+        <v>15</v>
+      </c>
+      <c r="R29" s="161">
+        <v>28</v>
+      </c>
+      <c r="S29" s="160">
+        <v>19</v>
+      </c>
+      <c r="T29" s="160">
+        <v>29</v>
+      </c>
+      <c r="U29" s="160">
+        <v>5</v>
+      </c>
+      <c r="V29" s="160">
+        <v>4</v>
+      </c>
+      <c r="W29" s="162">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update box locations on isolates
</commit_message>
<xml_diff>
--- a/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
+++ b/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah 23\Desktop\LabDocuments\FungalCulture\VdIsolatesList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFA51C5-E2EE-488A-B873-C423E352D139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD5CBF8-CAD9-4FE5-9A84-DBC740B1C92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8587" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8574" uniqueCount="1405">
   <si>
     <t>Plate</t>
   </si>
@@ -33644,8 +33644,8 @@
   <dimension ref="A1:H1135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35026,8 +35026,8 @@
       <c r="D68" s="17">
         <v>1996</v>
       </c>
-      <c r="E68" t="s">
-        <v>1364</v>
+      <c r="E68">
+        <v>3</v>
       </c>
       <c r="F68" t="s">
         <v>1401</v>
@@ -35046,8 +35046,8 @@
       <c r="D69" s="17">
         <v>1996</v>
       </c>
-      <c r="E69" t="s">
-        <v>1364</v>
+      <c r="E69">
+        <v>3</v>
       </c>
       <c r="F69" t="s">
         <v>1401</v>
@@ -35066,8 +35066,8 @@
       <c r="D70" s="16">
         <v>1996</v>
       </c>
-      <c r="E70" t="s">
-        <v>1364</v>
+      <c r="E70">
+        <v>3</v>
       </c>
       <c r="F70" t="s">
         <v>1401</v>
@@ -35086,8 +35086,8 @@
       <c r="D71" s="17">
         <v>1996</v>
       </c>
-      <c r="E71" t="s">
-        <v>1364</v>
+      <c r="E71">
+        <v>3</v>
       </c>
       <c r="F71" t="s">
         <v>1401</v>
@@ -35106,8 +35106,8 @@
       <c r="D72" s="17">
         <v>1996</v>
       </c>
-      <c r="E72" t="s">
-        <v>1364</v>
+      <c r="E72">
+        <v>3</v>
       </c>
       <c r="F72" t="s">
         <v>1401</v>
@@ -35284,8 +35284,8 @@
       <c r="D80" s="17">
         <v>1996</v>
       </c>
-      <c r="E80" t="s">
-        <v>1364</v>
+      <c r="E80">
+        <v>3</v>
       </c>
       <c r="F80" t="s">
         <v>1401</v>
@@ -35327,8 +35327,8 @@
       <c r="D82" s="16">
         <v>1996</v>
       </c>
-      <c r="E82" t="s">
-        <v>1364</v>
+      <c r="E82">
+        <v>3</v>
       </c>
       <c r="F82" t="s">
         <v>1401</v>
@@ -35347,8 +35347,8 @@
       <c r="D83" s="16">
         <v>1996</v>
       </c>
-      <c r="E83" t="s">
-        <v>1364</v>
+      <c r="E83">
+        <v>3</v>
       </c>
       <c r="F83" t="s">
         <v>1401</v>
@@ -35367,8 +35367,8 @@
       <c r="D84" s="16">
         <v>1996</v>
       </c>
-      <c r="E84" t="s">
-        <v>1364</v>
+      <c r="E84">
+        <v>3</v>
       </c>
       <c r="F84" t="s">
         <v>1401</v>
@@ -35484,8 +35484,8 @@
       <c r="D90" s="17">
         <v>1996</v>
       </c>
-      <c r="E90" t="s">
-        <v>1364</v>
+      <c r="E90">
+        <v>3</v>
       </c>
       <c r="F90" t="s">
         <v>1401</v>
@@ -35601,8 +35601,8 @@
       <c r="D96" s="16">
         <v>1996</v>
       </c>
-      <c r="E96" t="s">
-        <v>1364</v>
+      <c r="E96">
+        <v>3</v>
       </c>
       <c r="F96" t="s">
         <v>1401</v>
@@ -35621,8 +35621,8 @@
       <c r="D97" s="16">
         <v>1996</v>
       </c>
-      <c r="E97" t="s">
-        <v>1364</v>
+      <c r="E97">
+        <v>3</v>
       </c>
       <c r="F97" t="s">
         <v>1401</v>
@@ -35641,8 +35641,8 @@
       <c r="D98" s="16">
         <v>1996</v>
       </c>
-      <c r="E98" t="s">
-        <v>1364</v>
+      <c r="E98">
+        <v>3</v>
       </c>
       <c r="F98" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
Update plated isolates from Oct 19th
</commit_message>
<xml_diff>
--- a/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
+++ b/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah 23\Desktop\LabDocuments\FungalCulture\VdIsolatesList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD5CBF8-CAD9-4FE5-9A84-DBC740B1C92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7DE695-0193-4795-BDED-B3922E15359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8574" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8662" uniqueCount="1413">
   <si>
     <t>Plate</t>
   </si>
@@ -4284,6 +4284,30 @@
   </si>
   <si>
     <t>Harvestrd</t>
+  </si>
+  <si>
+    <t>Same as above?</t>
+  </si>
+  <si>
+    <t>103 LOOSE (103.SS ?)</t>
+  </si>
+  <si>
+    <t>105.LOOSE (105.SS ?)</t>
+  </si>
+  <si>
+    <t>208.LOOSE (208.SS ?)</t>
+  </si>
+  <si>
+    <t>212 LOOSE (212.SS ?)</t>
+  </si>
+  <si>
+    <t>3.I.2010</t>
+  </si>
+  <si>
+    <t>401 LOOSE (401.SS ?)</t>
+  </si>
+  <si>
+    <t>404.LOOSE (404.ss)</t>
   </si>
 </sst>
 </file>
@@ -33644,8 +33668,8 @@
   <dimension ref="A1:H1135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E131" sqref="E131"/>
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F304" sqref="F304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34595,7 +34619,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="122">
         <v>66</v>
       </c>
@@ -34738,7 +34762,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="122">
         <v>73</v>
       </c>
@@ -34758,7 +34782,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="122">
         <v>74</v>
       </c>
@@ -34781,7 +34805,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="122">
         <v>77</v>
       </c>
@@ -34801,7 +34825,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="122">
         <v>78</v>
       </c>
@@ -34821,7 +34845,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="122">
         <v>79</v>
       </c>
@@ -34867,7 +34891,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="122">
         <v>82</v>
       </c>
@@ -34887,7 +34911,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="122">
         <v>84</v>
       </c>
@@ -35013,7 +35037,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="122">
         <v>96</v>
       </c>
@@ -35033,7 +35057,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="122">
         <v>97</v>
       </c>
@@ -35053,7 +35077,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="122">
         <v>98</v>
       </c>
@@ -35073,7 +35097,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="121">
         <v>101</v>
       </c>
@@ -35093,7 +35117,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="121">
         <v>102</v>
       </c>
@@ -35113,7 +35137,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="121">
         <v>103</v>
       </c>
@@ -35136,7 +35160,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="121">
         <v>104</v>
       </c>
@@ -35159,7 +35183,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="121">
         <v>105</v>
       </c>
@@ -35248,7 +35272,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="121">
         <v>111</v>
       </c>
@@ -35271,7 +35295,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="121">
         <v>112</v>
       </c>
@@ -35314,7 +35338,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="121">
         <v>114</v>
       </c>
@@ -35334,7 +35358,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="121">
         <v>115</v>
       </c>
@@ -35354,7 +35378,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="121">
         <v>116</v>
       </c>
@@ -35397,7 +35421,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="121">
         <v>121</v>
       </c>
@@ -35417,7 +35441,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="121">
         <v>124</v>
       </c>
@@ -35471,7 +35495,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="121">
         <v>128</v>
       </c>
@@ -35491,7 +35515,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="121">
         <v>129</v>
       </c>
@@ -35511,7 +35535,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="121">
         <v>130</v>
       </c>
@@ -35588,7 +35612,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="121">
         <v>141</v>
       </c>
@@ -35608,7 +35632,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="121">
         <v>142</v>
       </c>
@@ -35628,7 +35652,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="121">
         <v>145</v>
       </c>
@@ -35665,7 +35689,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="121">
         <v>151</v>
       </c>
@@ -35685,7 +35709,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="121">
         <v>155</v>
       </c>
@@ -35740,7 +35764,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="119">
         <v>233</v>
       </c>
@@ -35760,7 +35784,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="119">
         <v>235</v>
       </c>
@@ -35783,7 +35807,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="119">
         <v>239</v>
       </c>
@@ -35806,7 +35830,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="119">
         <v>240</v>
       </c>
@@ -35860,7 +35884,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="129">
         <v>318</v>
       </c>
@@ -35897,7 +35921,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="129">
         <v>461</v>
       </c>
@@ -36073,7 +36097,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="129">
         <v>601</v>
       </c>
@@ -36093,7 +36117,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="119">
         <v>653</v>
       </c>
@@ -36141,7 +36165,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="138" t="s">
         <v>1036</v>
       </c>
@@ -36152,7 +36176,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="123" t="s">
         <v>539</v>
       </c>
@@ -36166,7 +36190,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="123" t="s">
         <v>42</v>
       </c>
@@ -36182,8 +36206,11 @@
       <c r="E131" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F131" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="123" t="s">
         <v>1376</v>
       </c>
@@ -36197,8 +36224,11 @@
       <c r="E132" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F132" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="143" t="s">
         <v>1377</v>
       </c>
@@ -36214,8 +36244,11 @@
       <c r="E133" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F133" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="123" t="s">
         <v>164</v>
       </c>
@@ -36229,8 +36262,11 @@
       <c r="E134" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F134" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="123" t="s">
         <v>170</v>
       </c>
@@ -36244,8 +36280,11 @@
       <c r="E135" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F135" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
         <v>134</v>
       </c>
@@ -36262,7 +36301,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
         <v>137</v>
       </c>
@@ -36279,7 +36318,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
         <v>138</v>
       </c>
@@ -36296,7 +36335,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
         <v>154</v>
       </c>
@@ -36313,7 +36352,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
         <v>155</v>
       </c>
@@ -36330,7 +36369,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
         <v>139</v>
       </c>
@@ -36347,7 +36386,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="124" t="s">
         <v>945</v>
       </c>
@@ -36364,7 +36403,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="124" t="s">
         <v>944</v>
       </c>
@@ -36381,7 +36420,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="124" t="s">
         <v>943</v>
       </c>
@@ -36398,7 +36437,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="124" t="s">
         <v>940</v>
       </c>
@@ -36415,7 +36454,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="124" t="s">
         <v>941</v>
       </c>
@@ -36432,7 +36471,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="124" t="s">
         <v>942</v>
       </c>
@@ -36449,7 +36488,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="123" t="s">
         <v>214</v>
       </c>
@@ -36465,8 +36504,11 @@
       <c r="E148" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F148" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="123" t="s">
         <v>211</v>
       </c>
@@ -36482,8 +36524,11 @@
       <c r="E149" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F149" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="123" t="s">
         <v>215</v>
       </c>
@@ -36499,8 +36544,11 @@
       <c r="E150" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F150" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="124" t="s">
         <v>954</v>
       </c>
@@ -36517,7 +36565,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="123" t="s">
         <v>261</v>
       </c>
@@ -36533,8 +36581,11 @@
       <c r="E152" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F152" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="124" t="s">
         <v>951</v>
       </c>
@@ -36551,7 +36602,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="124" t="s">
         <v>953</v>
       </c>
@@ -36568,7 +36619,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="124" t="s">
         <v>953</v>
       </c>
@@ -36585,7 +36636,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="124" t="s">
         <v>955</v>
       </c>
@@ -36602,7 +36653,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="124" t="s">
         <v>955</v>
       </c>
@@ -36619,7 +36670,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="123" t="s">
         <v>264</v>
       </c>
@@ -36635,8 +36686,11 @@
       <c r="E158" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F158" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
         <v>262</v>
       </c>
@@ -36653,7 +36707,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="123" t="s">
         <v>212</v>
       </c>
@@ -36669,8 +36723,11 @@
       <c r="E160" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F160" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="124" t="s">
         <v>958</v>
       </c>
@@ -36687,7 +36744,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="124" t="s">
         <v>956</v>
       </c>
@@ -36704,7 +36761,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="135" t="s">
         <v>1019</v>
       </c>
@@ -36720,8 +36777,11 @@
       <c r="E163" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F163" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="123" t="s">
         <v>265</v>
       </c>
@@ -36737,8 +36797,11 @@
       <c r="E164" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F164" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="124" t="s">
         <v>948</v>
       </c>
@@ -36755,7 +36818,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="124" t="s">
         <v>950</v>
       </c>
@@ -36772,7 +36835,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="123" t="s">
         <v>216</v>
       </c>
@@ -36788,8 +36851,11 @@
       <c r="E167" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F167" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="123" t="s">
         <v>266</v>
       </c>
@@ -36805,8 +36871,11 @@
       <c r="E168" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F168" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="123" t="s">
         <v>267</v>
       </c>
@@ -36822,8 +36891,11 @@
       <c r="E169" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F169" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="123" t="s">
         <v>218</v>
       </c>
@@ -36839,8 +36911,11 @@
       <c r="E170" s="39" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F170" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="124" t="s">
         <v>1320</v>
       </c>
@@ -36851,7 +36926,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="123" t="s">
         <v>345</v>
       </c>
@@ -36867,8 +36942,11 @@
       <c r="E172" s="39" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F172" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="123" t="s">
         <v>347</v>
       </c>
@@ -36884,10 +36962,13 @@
       <c r="E173" s="39" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F173" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="132" t="s">
-        <v>320</v>
+        <v>1406</v>
       </c>
       <c r="B174" s="62" t="s">
         <v>165</v>
@@ -36899,12 +36980,15 @@
         <v>2010</v>
       </c>
       <c r="E174" s="39" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+      <c r="F174" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="132" t="s">
-        <v>326</v>
+        <v>1407</v>
       </c>
       <c r="B175" s="62" t="s">
         <v>165</v>
@@ -36916,10 +37000,13 @@
         <v>2010</v>
       </c>
       <c r="E175" s="39" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+      <c r="F175" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="132" t="s">
         <v>327</v>
       </c>
@@ -36933,7 +37020,10 @@
         <v>2010</v>
       </c>
       <c r="E176" s="39" t="s">
-        <v>1367</v>
+        <v>1364</v>
+      </c>
+      <c r="F176" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -36991,6 +37081,9 @@
       <c r="E180" s="39" t="s">
         <v>1364</v>
       </c>
+      <c r="F180" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="181" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="123" t="s">
@@ -37008,6 +37101,9 @@
       <c r="E181" t="s">
         <v>1372</v>
       </c>
+      <c r="F181" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="182" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="124" t="s">
@@ -37047,6 +37143,9 @@
       <c r="E184" t="s">
         <v>1374</v>
       </c>
+      <c r="F184" t="s">
+        <v>1401</v>
+      </c>
       <c r="G184" t="s">
         <v>1400</v>
       </c>
@@ -37067,6 +37166,9 @@
       <c r="E185" t="s">
         <v>1371</v>
       </c>
+      <c r="F185" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="186" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="124" t="s">
@@ -37117,6 +37219,9 @@
       <c r="E189" t="s">
         <v>1364</v>
       </c>
+      <c r="F189" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="190" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="124" t="s">
@@ -37145,6 +37250,9 @@
       <c r="E191" t="s">
         <v>1374</v>
       </c>
+      <c r="F191" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="192" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="131" t="s">
@@ -37162,6 +37270,9 @@
       <c r="E192" t="s">
         <v>1374</v>
       </c>
+      <c r="F192" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="193" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="123" t="s">
@@ -37177,7 +37288,10 @@
         <v>2008</v>
       </c>
       <c r="E193" t="s">
-        <v>1374</v>
+        <v>1372</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -37207,6 +37321,9 @@
       <c r="E195" t="s">
         <v>1374</v>
       </c>
+      <c r="F195" t="s">
+        <v>1401</v>
+      </c>
       <c r="G195" t="s">
         <v>1400</v>
       </c>
@@ -37238,6 +37355,9 @@
       <c r="E197" t="s">
         <v>1374</v>
       </c>
+      <c r="F197" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="198" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="131" t="s">
@@ -37255,6 +37375,9 @@
       <c r="E198" t="s">
         <v>1374</v>
       </c>
+      <c r="F198" t="s">
+        <v>1401</v>
+      </c>
       <c r="G198" t="s">
         <v>1400</v>
       </c>
@@ -37292,6 +37415,9 @@
       <c r="E200" t="s">
         <v>1374</v>
       </c>
+      <c r="F200" t="s">
+        <v>1401</v>
+      </c>
       <c r="G200" t="s">
         <v>1400</v>
       </c>
@@ -37315,7 +37441,7 @@
     </row>
     <row r="202" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="132" t="s">
-        <v>319</v>
+        <v>1408</v>
       </c>
       <c r="B202" s="62" t="s">
         <v>165</v>
@@ -37327,7 +37453,10 @@
         <v>2010</v>
       </c>
       <c r="E202" t="s">
-        <v>1374</v>
+        <v>1367</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -37391,6 +37520,9 @@
       <c r="E206" t="s">
         <v>1374</v>
       </c>
+      <c r="F206" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="207" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="132" t="s">
@@ -37408,6 +37540,9 @@
       <c r="E207" t="s">
         <v>1374</v>
       </c>
+      <c r="F207" t="s">
+        <v>1401</v>
+      </c>
       <c r="G207" t="s">
         <v>1400</v>
       </c>
@@ -37428,6 +37563,9 @@
       <c r="E208" t="s">
         <v>1374</v>
       </c>
+      <c r="F208" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="209" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="131" t="s">
@@ -37445,6 +37583,9 @@
       <c r="E209" t="s">
         <v>1374</v>
       </c>
+      <c r="F209" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="210" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="131" t="s">
@@ -37462,6 +37603,9 @@
       <c r="E210" t="s">
         <v>1374</v>
       </c>
+      <c r="F210" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="211" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="123" t="s">
@@ -37479,10 +37623,13 @@
       <c r="E211" t="s">
         <v>1372</v>
       </c>
+      <c r="F211" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="212" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="132" t="s">
-        <v>324</v>
+        <v>1409</v>
       </c>
       <c r="B212" s="62" t="s">
         <v>165</v>
@@ -37495,6 +37642,9 @@
       </c>
       <c r="E212" t="s">
         <v>1367</v>
+      </c>
+      <c r="F212" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -37535,6 +37685,9 @@
       <c r="E215" t="s">
         <v>1374</v>
       </c>
+      <c r="F215" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="216" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="119" t="s">
@@ -37552,6 +37705,9 @@
       <c r="E216" t="s">
         <v>1367</v>
       </c>
+      <c r="F216" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="217" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="131" t="s">
@@ -37586,13 +37742,16 @@
       <c r="E218" t="s">
         <v>1374</v>
       </c>
+      <c r="F218" t="s">
+        <v>1401</v>
+      </c>
       <c r="G218" t="s">
         <v>1400</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="131" t="s">
-        <v>239</v>
+        <v>1410</v>
       </c>
       <c r="B219" s="55" t="s">
         <v>165</v>
@@ -37605,6 +37764,9 @@
       </c>
       <c r="E219" t="s">
         <v>1374</v>
+      </c>
+      <c r="F219" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -37667,6 +37829,9 @@
       <c r="E224" t="s">
         <v>1374</v>
       </c>
+      <c r="F224" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="225" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="131" t="s">
@@ -37684,6 +37849,9 @@
       <c r="E225" t="s">
         <v>1374</v>
       </c>
+      <c r="F225" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="226" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="123" t="s">
@@ -37701,6 +37869,9 @@
       <c r="E226" t="s">
         <v>1372</v>
       </c>
+      <c r="F226" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="227" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="124" t="s">
@@ -37729,6 +37900,9 @@
       <c r="E228" t="s">
         <v>1374</v>
       </c>
+      <c r="F228" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="229" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229" s="131" t="s">
@@ -37746,6 +37920,9 @@
       <c r="E229" t="s">
         <v>1374</v>
       </c>
+      <c r="F229" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="230" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="131" t="s">
@@ -37763,6 +37940,9 @@
       <c r="E230" t="s">
         <v>1374</v>
       </c>
+      <c r="F230" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="231" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="130" t="s">
@@ -37780,10 +37960,13 @@
       <c r="E231" t="s">
         <v>1374</v>
       </c>
+      <c r="F231" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="232" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="132" t="s">
-        <v>325</v>
+        <v>1411</v>
       </c>
       <c r="B232" s="62" t="s">
         <v>165</v>
@@ -37796,6 +37979,9 @@
       </c>
       <c r="E232" t="s">
         <v>1367</v>
+      </c>
+      <c r="F232" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -37814,10 +38000,13 @@
       <c r="E233" t="s">
         <v>1367</v>
       </c>
+      <c r="F233" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="234" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="132" t="s">
-        <v>316</v>
+        <v>1412</v>
       </c>
       <c r="B234" s="62" t="s">
         <v>165</v>
@@ -37830,6 +38019,9 @@
       </c>
       <c r="E234" t="s">
         <v>1367</v>
+      </c>
+      <c r="F234" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="235" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -37848,6 +38040,9 @@
       <c r="E235" t="s">
         <v>1367</v>
       </c>
+      <c r="F235" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="236" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="131" t="s">
@@ -37865,6 +38060,9 @@
       <c r="E236" t="s">
         <v>1374</v>
       </c>
+      <c r="F236" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="237" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="133" t="s">
@@ -37882,6 +38080,9 @@
       <c r="E237" t="s">
         <v>1374</v>
       </c>
+      <c r="F237" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="238" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="131" t="s">
@@ -37899,6 +38100,9 @@
       <c r="E238" t="s">
         <v>1374</v>
       </c>
+      <c r="F238" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="239" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="131" t="s">
@@ -37916,6 +38120,9 @@
       <c r="E239" t="s">
         <v>1374</v>
       </c>
+      <c r="F239" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="240" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="133" t="s">
@@ -37933,6 +38140,9 @@
       <c r="E240" t="s">
         <v>1374</v>
       </c>
+      <c r="F240" t="s">
+        <v>1401</v>
+      </c>
       <c r="G240" t="s">
         <v>1400</v>
       </c>
@@ -37953,6 +38163,9 @@
       <c r="E241" t="s">
         <v>1372</v>
       </c>
+      <c r="F241" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="242" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="124" t="s">
@@ -38043,6 +38256,9 @@
       <c r="E247" t="s">
         <v>1374</v>
       </c>
+      <c r="F247" t="s">
+        <v>1401</v>
+      </c>
       <c r="G247" t="s">
         <v>1400</v>
       </c>
@@ -38063,6 +38279,9 @@
       <c r="E248" t="s">
         <v>1374</v>
       </c>
+      <c r="F248" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="249" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249" s="131" t="s">
@@ -38080,6 +38299,9 @@
       <c r="E249" t="s">
         <v>1374</v>
       </c>
+      <c r="F249" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="250" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A250" s="131" t="s">
@@ -38097,6 +38319,9 @@
       <c r="E250" t="s">
         <v>1374</v>
       </c>
+      <c r="F250" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="251" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="131" t="s">
@@ -38114,6 +38339,9 @@
       <c r="E251" t="s">
         <v>1374</v>
       </c>
+      <c r="F251" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="252" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="124" t="s">
@@ -38142,6 +38370,9 @@
       <c r="E253" t="s">
         <v>1374</v>
       </c>
+      <c r="F253" t="s">
+        <v>1401</v>
+      </c>
       <c r="G253" t="s">
         <v>1400</v>
       </c>
@@ -38162,6 +38393,9 @@
       <c r="E254" t="s">
         <v>1374</v>
       </c>
+      <c r="F254" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="255" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A255" s="123" t="s">
@@ -38179,6 +38413,9 @@
       <c r="E255" t="s">
         <v>1372</v>
       </c>
+      <c r="F255" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="256" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A256" s="123" t="s">
@@ -38196,8 +38433,11 @@
       <c r="E256" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F256" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="29" t="s">
         <v>75</v>
       </c>
@@ -38214,7 +38454,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="258" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A258" s="123" t="s">
         <v>329</v>
       </c>
@@ -38228,8 +38468,11 @@
       <c r="E258" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F258" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="123" t="s">
         <v>372</v>
       </c>
@@ -38246,7 +38489,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="124" t="s">
         <v>1145</v>
       </c>
@@ -38257,7 +38500,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="124" t="s">
         <v>1134</v>
       </c>
@@ -38268,7 +38511,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A262" s="123" t="s">
         <v>355</v>
       </c>
@@ -38284,8 +38527,11 @@
       <c r="E262" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F262" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A263" s="123" t="s">
         <v>185</v>
       </c>
@@ -38301,8 +38547,11 @@
       <c r="E263" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="264" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F263" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="124" t="s">
         <v>1223</v>
       </c>
@@ -38316,7 +38565,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="124" t="s">
         <v>1222</v>
       </c>
@@ -38330,7 +38579,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="124" t="s">
         <v>1224</v>
       </c>
@@ -38344,7 +38593,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="124" t="s">
         <v>1225</v>
       </c>
@@ -38358,7 +38607,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="124" t="s">
         <v>1226</v>
       </c>
@@ -38372,7 +38621,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="124" t="s">
         <v>1227</v>
       </c>
@@ -38386,7 +38635,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="270" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="124" t="s">
         <v>1228</v>
       </c>
@@ -38400,7 +38649,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="124" t="s">
         <v>1229</v>
       </c>
@@ -38414,7 +38663,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="124" t="s">
         <v>1230</v>
       </c>
@@ -38428,7 +38677,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="273" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="124" t="s">
         <v>1231</v>
       </c>
@@ -38442,7 +38691,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="124" t="s">
         <v>1310</v>
       </c>
@@ -38456,7 +38705,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="275" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="124" t="s">
         <v>1311</v>
       </c>
@@ -38470,7 +38719,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="124" t="s">
         <v>1124</v>
       </c>
@@ -38481,7 +38730,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="124" t="s">
         <v>1111</v>
       </c>
@@ -38492,7 +38741,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="278" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="124" t="s">
         <v>1157</v>
       </c>
@@ -38503,7 +38752,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="279" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="124" t="s">
         <v>1123</v>
       </c>
@@ -38514,7 +38763,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="124" t="s">
         <v>1144</v>
       </c>
@@ -38525,7 +38774,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="281" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="124" t="s">
         <v>996</v>
       </c>
@@ -38542,7 +38791,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="282" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A282" s="123" t="s">
         <v>363</v>
       </c>
@@ -38556,8 +38805,11 @@
       <c r="E282" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="283" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F282" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A283" s="123" t="s">
         <v>213</v>
       </c>
@@ -38573,8 +38825,11 @@
       <c r="E283" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="284" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F283" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="128" t="s">
         <v>149</v>
       </c>
@@ -38591,7 +38846,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="124" t="s">
         <v>1115</v>
       </c>
@@ -38602,7 +38857,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="124" t="s">
         <v>1125</v>
       </c>
@@ -38613,7 +38868,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="287" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="124" t="s">
         <v>1125</v>
       </c>
@@ -38624,7 +38879,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="288" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="124" t="s">
         <v>1347</v>
       </c>
@@ -38635,7 +38890,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="289" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="124" t="s">
         <v>1346</v>
       </c>
@@ -38646,7 +38901,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="290" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="124" t="s">
         <v>1348</v>
       </c>
@@ -38657,7 +38912,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="291" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="124" t="s">
         <v>1344</v>
       </c>
@@ -38668,7 +38923,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="292" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="124" t="s">
         <v>1345</v>
       </c>
@@ -38679,7 +38934,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="293" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="120" t="s">
         <v>430</v>
       </c>
@@ -38696,7 +38951,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="294" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A294" s="123" t="s">
         <v>303</v>
       </c>
@@ -38712,8 +38967,11 @@
       <c r="E294" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="295" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F294" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A295" s="123" t="s">
         <v>376</v>
       </c>
@@ -38729,8 +38987,11 @@
       <c r="E295" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="296" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F295" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A296" s="123" t="s">
         <v>306</v>
       </c>
@@ -38746,8 +39007,11 @@
       <c r="E296" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="297" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F296" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A297" s="123" t="s">
         <v>297</v>
       </c>
@@ -38763,8 +39027,11 @@
       <c r="E297" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="298" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F297" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="123" t="s">
         <v>302</v>
       </c>
@@ -38780,8 +39047,11 @@
       <c r="E298" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="299" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F298" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="123" t="s">
         <v>291</v>
       </c>
@@ -38797,8 +39067,11 @@
       <c r="E299" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="300" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F299" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A300" s="123" t="s">
         <v>397</v>
       </c>
@@ -38814,8 +39087,11 @@
       <c r="E300" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="301" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F300" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A301" s="123" t="s">
         <v>367</v>
       </c>
@@ -38831,8 +39107,11 @@
       <c r="E301" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F301" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A302" s="123" t="s">
         <v>293</v>
       </c>
@@ -38848,8 +39127,11 @@
       <c r="E302" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="303" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F302" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A303" s="123" t="s">
         <v>368</v>
       </c>
@@ -38865,8 +39147,11 @@
       <c r="E303" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="304" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F303" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A304" s="123" t="s">
         <v>285</v>
       </c>
@@ -38881,6 +39166,9 @@
       </c>
       <c r="E304" t="s">
         <v>1375</v>
+      </c>
+      <c r="F304" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="305" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -42093,7 +42381,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="555" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" s="127" t="s">
         <v>627</v>
       </c>
@@ -42149,7 +42437,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="559" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" s="127" t="s">
         <v>648</v>
       </c>
@@ -42183,7 +42471,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="561" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561" s="127" t="s">
         <v>619</v>
       </c>
@@ -42217,7 +42505,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="563" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" s="127" t="s">
         <v>661</v>
       </c>
@@ -42342,7 +42630,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="570" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A570" s="127" t="s">
         <v>645</v>
       </c>
@@ -42356,7 +42644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="571" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571" s="127" t="s">
         <v>644</v>
       </c>
@@ -42390,7 +42678,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="573" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A573" s="127" t="s">
         <v>616</v>
       </c>
@@ -42404,7 +42692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="574" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A574" s="127" t="s">
         <v>651</v>
       </c>
@@ -46506,7 +46794,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="868" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A868" s="127" t="s">
         <v>625</v>
       </c>
@@ -46520,7 +46808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="869" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A869" s="127" t="s">
         <v>626</v>
       </c>
@@ -46534,7 +46822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="870" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A870" s="127" t="s">
         <v>632</v>
       </c>
@@ -46568,7 +46856,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="872" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A872" s="126" t="s">
         <v>553</v>
       </c>
@@ -46579,7 +46867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="873" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A873" s="127" t="s">
         <v>629</v>
       </c>
@@ -46593,7 +46881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="874" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A874" s="127" t="s">
         <v>630</v>
       </c>
@@ -46607,7 +46895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="875" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A875" s="127" t="s">
         <v>635</v>
       </c>
@@ -46695,7 +46983,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="880" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A880" s="127" t="s">
         <v>646</v>
       </c>
@@ -46709,7 +46997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="881" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A881" s="127" t="s">
         <v>647</v>
       </c>
@@ -46777,7 +47065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="885" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A885" s="127" t="s">
         <v>649</v>
       </c>
@@ -46887,7 +47175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="892" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A892" s="127" t="s">
         <v>658</v>
       </c>
@@ -46901,7 +47189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="893" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A893" s="127" t="s">
         <v>659</v>
       </c>
@@ -46915,7 +47203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="894" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A894" s="127" t="s">
         <v>662</v>
       </c>
@@ -46954,7 +47242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="897" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A897" s="127" t="s">
         <v>664</v>
       </c>
@@ -46968,7 +47256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="898" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A898" s="127" t="s">
         <v>665</v>
       </c>
@@ -47033,7 +47321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="902" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902" s="127" t="s">
         <v>667</v>
       </c>
@@ -47058,7 +47346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="904" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A904" s="127" t="s">
         <v>623</v>
       </c>
@@ -47092,7 +47380,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="906" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A906" s="127" t="s">
         <v>624</v>
       </c>
@@ -47126,7 +47414,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="908" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A908" s="127" t="s">
         <v>621</v>
       </c>
@@ -47162,7 +47450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="911" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A911" s="127" t="s">
         <v>670</v>
       </c>
@@ -47204,7 +47492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="914" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A914" s="127" t="s">
         <v>672</v>
       </c>
@@ -47218,7 +47506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="915" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A915" s="127" t="s">
         <v>673</v>
       </c>
@@ -47286,7 +47574,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="919" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A919" s="127" t="s">
         <v>676</v>
       </c>
@@ -47418,7 +47706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="928" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A928" s="127" t="s">
         <v>575</v>
       </c>
@@ -47432,7 +47720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="929" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A929" s="127" t="s">
         <v>574</v>
       </c>
@@ -49379,7 +49667,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1061" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1061" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1061" s="127" t="s">
         <v>571</v>
       </c>
@@ -49413,7 +49701,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1063" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1063" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1063" s="127" t="s">
         <v>671</v>
       </c>
@@ -49822,7 +50110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1086" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1086" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1086" s="127" t="s">
         <v>587</v>
       </c>
@@ -49862,7 +50150,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1088" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1088" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1088" s="127" t="s">
         <v>582</v>
       </c>
@@ -49932,7 +50220,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1093" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1093" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1093" s="127" t="s">
         <v>569</v>
       </c>
@@ -50072,7 +50360,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1103" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1103" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1103" s="127" t="s">
         <v>668</v>
       </c>
@@ -50108,7 +50396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1106" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1106" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1106" s="127" t="s">
         <v>669</v>
       </c>
@@ -50144,7 +50432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1109" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1109" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1109" s="127" t="s">
         <v>675</v>
       </c>
@@ -50172,7 +50460,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1111" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1111" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1111" s="127" t="s">
         <v>606</v>
       </c>
@@ -50306,7 +50594,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="1118" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1118" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1118" s="127" t="s">
         <v>581</v>
       </c>
@@ -50596,7 +50884,6 @@
         <filter val="2G"/>
         <filter val="2H"/>
         <filter val="3"/>
-        <filter val="4"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">

</xml_diff>

<commit_message>
Update plated isolates for Oct 22nd
</commit_message>
<xml_diff>
--- a/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
+++ b/FungalCulture/VdIsolatesList/Organized Vd_list_JKSD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah 23\Desktop\LabDocuments\FungalCulture\VdIsolatesList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D014DDE-B1D6-4A3D-A05F-0D7D96BD82A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C242417E-6984-497C-ADC8-2337D681FFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9433" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9484" uniqueCount="1413">
   <si>
     <t>Plate</t>
   </si>
@@ -4305,6 +4305,9 @@
   </si>
   <si>
     <t>Same as above?</t>
+  </si>
+  <si>
+    <t>Same as LS8A?</t>
   </si>
 </sst>
 </file>
@@ -5068,56 +5071,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -33714,8 +33668,8 @@
   <dimension ref="A1:H1136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F239" sqref="F239"/>
+      <pane ySplit="1" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F239" sqref="F239:F1136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38359,6 +38313,9 @@
       <c r="E239" t="s">
         <v>1375</v>
       </c>
+      <c r="F239" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="240" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="123" t="s">
@@ -38376,6 +38333,9 @@
       <c r="E240" t="s">
         <v>1375</v>
       </c>
+      <c r="F240" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="241" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="123" t="s">
@@ -38393,6 +38353,9 @@
       <c r="E241" t="s">
         <v>1375</v>
       </c>
+      <c r="F241" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="242" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="124" t="s">
@@ -38498,6 +38461,9 @@
       <c r="E247" t="s">
         <v>1375</v>
       </c>
+      <c r="F247" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="248" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A248" s="123" t="s">
@@ -38515,6 +38481,9 @@
       <c r="E248" t="s">
         <v>1375</v>
       </c>
+      <c r="F248" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="249" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249" s="123" t="s">
@@ -38532,6 +38501,9 @@
       <c r="E249" t="s">
         <v>1375</v>
       </c>
+      <c r="F249" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="250" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A250" s="123" t="s">
@@ -38549,6 +38521,9 @@
       <c r="E250" t="s">
         <v>1384</v>
       </c>
+      <c r="F250" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="251" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="123" t="s">
@@ -38566,6 +38541,9 @@
       <c r="E251" t="s">
         <v>1384</v>
       </c>
+      <c r="F251" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="252" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="124" t="s">
@@ -38597,6 +38575,9 @@
       <c r="E253" t="s">
         <v>1384</v>
       </c>
+      <c r="F253" t="s">
+        <v>1401</v>
+      </c>
       <c r="G253" t="s">
         <v>1400</v>
       </c>
@@ -38617,6 +38598,9 @@
       <c r="E254" t="s">
         <v>1384</v>
       </c>
+      <c r="F254" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="255" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A255" s="123" t="s">
@@ -38634,6 +38618,9 @@
       <c r="E255" t="s">
         <v>1384</v>
       </c>
+      <c r="F255" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="256" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A256" s="120" t="s">
@@ -38651,6 +38638,9 @@
       <c r="E256" t="s">
         <v>1384</v>
       </c>
+      <c r="F256" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="257" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A257" s="123" t="s">
@@ -38668,6 +38658,9 @@
       <c r="E257" t="s">
         <v>1384</v>
       </c>
+      <c r="F257" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="258" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A258" s="123" t="s">
@@ -38685,6 +38678,9 @@
       <c r="E258" t="s">
         <v>1384</v>
       </c>
+      <c r="F258" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="259" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="123" t="s">
@@ -38750,6 +38746,9 @@
       <c r="E262" t="s">
         <v>1384</v>
       </c>
+      <c r="F262" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="263" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A263" s="123" t="s">
@@ -38767,6 +38766,9 @@
       <c r="E263" t="s">
         <v>1384</v>
       </c>
+      <c r="F263" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="264" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="124" t="s">
@@ -39078,6 +39080,9 @@
       <c r="E282" t="s">
         <v>1384</v>
       </c>
+      <c r="F282" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="283" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A283" s="123" t="s">
@@ -39095,6 +39100,9 @@
       <c r="E283" t="s">
         <v>1384</v>
       </c>
+      <c r="F283" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="284" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="128" t="s">
@@ -39264,6 +39272,9 @@
       <c r="E294" t="s">
         <v>1384</v>
       </c>
+      <c r="F294" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="295" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A295" s="123" t="s">
@@ -39281,6 +39292,9 @@
       <c r="E295" t="s">
         <v>1384</v>
       </c>
+      <c r="F295" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="296" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A296" s="124" t="s">
@@ -39292,6 +39306,9 @@
       <c r="E296" t="s">
         <v>1384</v>
       </c>
+      <c r="F296" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="297" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A297" s="124" t="s">
@@ -39303,6 +39320,9 @@
       <c r="E297" t="s">
         <v>1384</v>
       </c>
+      <c r="F297" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="298" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="123" t="s">
@@ -39320,6 +39340,9 @@
       <c r="E298" t="s">
         <v>1373</v>
       </c>
+      <c r="F298" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="299" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="123" t="s">
@@ -39337,6 +39360,9 @@
       <c r="E299" t="s">
         <v>1373</v>
       </c>
+      <c r="F299" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="300" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A300" s="123" t="s">
@@ -39354,6 +39380,9 @@
       <c r="E300" t="s">
         <v>1390</v>
       </c>
+      <c r="F300" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="301" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A301" s="123" t="s">
@@ -39371,6 +39400,9 @@
       <c r="E301" t="s">
         <v>1390</v>
       </c>
+      <c r="F301" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="302" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A302" s="123" t="s">
@@ -39388,6 +39420,9 @@
       <c r="E302" t="s">
         <v>1390</v>
       </c>
+      <c r="F302" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="303" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A303" s="123" t="s">
@@ -39405,6 +39440,9 @@
       <c r="E303" t="s">
         <v>1391</v>
       </c>
+      <c r="F303" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="304" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A304" s="123" t="s">
@@ -39422,6 +39460,9 @@
       <c r="E304" t="s">
         <v>1391</v>
       </c>
+      <c r="F304" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="305" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A305" s="123" t="s">
@@ -39439,6 +39480,9 @@
       <c r="E305" t="s">
         <v>1391</v>
       </c>
+      <c r="F305" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="306" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A306" s="123" t="s">
@@ -39456,6 +39500,9 @@
       <c r="E306" t="s">
         <v>1391</v>
       </c>
+      <c r="F306" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="307" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A307" s="123" t="s">
@@ -39473,6 +39520,9 @@
       <c r="E307" t="s">
         <v>1391</v>
       </c>
+      <c r="F307" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="308" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A308" s="123" t="s">
@@ -39490,6 +39540,9 @@
       <c r="E308" t="s">
         <v>1391</v>
       </c>
+      <c r="F308" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="309" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="124" t="s">
@@ -39577,6 +39630,9 @@
       <c r="E314" t="s">
         <v>1391</v>
       </c>
+      <c r="F314" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="315" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="123" t="s">
@@ -42000,6 +42056,9 @@
       <c r="E468" t="s">
         <v>1392</v>
       </c>
+      <c r="F468" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="469" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" s="124" t="s">
@@ -42037,6 +42096,9 @@
       <c r="E470" t="s">
         <v>1392</v>
       </c>
+      <c r="F470" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="471" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A471" s="123" t="s">
@@ -42054,6 +42116,9 @@
       <c r="E471" t="s">
         <v>1392</v>
       </c>
+      <c r="F471" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="472" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A472" s="131" t="s">
@@ -42071,6 +42136,9 @@
       <c r="E472" t="s">
         <v>1392</v>
       </c>
+      <c r="F472" t="s">
+        <v>1401</v>
+      </c>
       <c r="G472" t="s">
         <v>1400</v>
       </c>
@@ -42111,6 +42179,9 @@
       <c r="E474" t="s">
         <v>1392</v>
       </c>
+      <c r="F474" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="475" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A475" s="123" t="s">
@@ -42128,6 +42199,9 @@
       <c r="E475" t="s">
         <v>1392</v>
       </c>
+      <c r="F475" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="476" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" s="124" t="s">
@@ -42937,7 +43011,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="533" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" s="124" t="s">
         <v>961</v>
       </c>
@@ -42946,7 +43020,7 @@
       </c>
       <c r="D533" s="118"/>
       <c r="E533" t="s">
-        <v>1385</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="534" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -42965,6 +43039,9 @@
       <c r="E534" t="s">
         <v>1392</v>
       </c>
+      <c r="F534" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="535" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" s="123" t="s">
@@ -43002,6 +43079,9 @@
       <c r="E536" t="s">
         <v>1392</v>
       </c>
+      <c r="F536" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="537" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A537" s="123" t="s">
@@ -43017,6 +43097,9 @@
       <c r="E537" t="s">
         <v>1392</v>
       </c>
+      <c r="F537" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="538" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" s="124" t="s">
@@ -43128,6 +43211,9 @@
       <c r="E543" t="s">
         <v>1392</v>
       </c>
+      <c r="F543" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="544" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" s="124" t="s">
@@ -43162,6 +43248,9 @@
       <c r="E545" t="s">
         <v>1392</v>
       </c>
+      <c r="F545" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="546" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A546" s="123" t="s">
@@ -43179,6 +43268,9 @@
       <c r="E546" t="s">
         <v>1392</v>
       </c>
+      <c r="F546" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="547" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A547" s="123" t="s">
@@ -43196,6 +43288,9 @@
       <c r="E547" t="s">
         <v>1392</v>
       </c>
+      <c r="F547" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="548" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" s="124" t="s">
@@ -43233,6 +43328,9 @@
       <c r="E549" t="s">
         <v>1392</v>
       </c>
+      <c r="F549" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="550" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" s="124" t="s">
@@ -43284,6 +43382,9 @@
       <c r="E552" t="s">
         <v>1392</v>
       </c>
+      <c r="F552" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="553" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A553" s="123" t="s">
@@ -43301,6 +43402,9 @@
       <c r="E553" t="s">
         <v>1392</v>
       </c>
+      <c r="F553" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="554" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554" s="28">
@@ -47405,7 +47509,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="791" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A791" s="139" t="s">
         <v>1200</v>
       </c>
@@ -47420,6 +47524,9 @@
       </c>
       <c r="E791" t="s">
         <v>1384</v>
+      </c>
+      <c r="F791" t="s">
+        <v>1412</v>
       </c>
     </row>
     <row r="792" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>